<commit_message>
Conclusiones, mediciones cargadas y cuentas...
</commit_message>
<xml_diff>
--- a/EJ3/Mediciones/Actuales/Plantilla_Mediciones.xlsx
+++ b/EJ3/Mediciones/Actuales/Plantilla_Mediciones.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Nº</t>
   </si>
@@ -217,6 +217,18 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>Medir las tensiones de alimentación en ambos casos límite de la frecuencia</t>
+  </si>
+  <si>
+    <t>Usando dos canales, medir VCC y VEE, para ambos casos de frecuencias.</t>
+  </si>
+  <si>
+    <t>Observar si los picos son distintos, culpa de un mal desacople, produce asimetría en la alimentación del amplificador operacional.</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -449,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -476,9 +488,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -830,7 +839,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,10 +874,10 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="18"/>
+      <c r="H1" s="17"/>
       <c r="J1" s="7" t="s">
         <v>7</v>
       </c>
@@ -877,7 +886,7 @@
       <c r="A2" s="3">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -886,14 +895,14 @@
       <c r="D2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>23</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20"/>
+        <v>10</v>
+      </c>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
@@ -901,21 +910,23 @@
         <f>A2+1</f>
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="16"/>
+      <c r="E3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="15"/>
       <c r="J3" s="5" t="s">
         <v>11</v>
       </c>
@@ -925,21 +936,23 @@
         <f t="shared" ref="A4:A6" si="0">A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="16"/>
+      <c r="E4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
       <c r="J4" s="5" t="s">
         <v>12</v>
       </c>
@@ -949,7 +962,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -958,28 +971,40 @@
       <c r="D5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="16"/>
+      <c r="E5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="15"/>
       <c r="J5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
+      <c r="B6" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15"/>
       <c r="J6" s="5" t="s">
         <v>9</v>
       </c>

</xml_diff>